<commit_message>
Aggregrated now gives only 2014 data for certain selected countries
</commit_message>
<xml_diff>
--- a/output/SDN.xlsx
+++ b/output/SDN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>0. Crop yield (Wheat, tons)</t>
+          <t>0. Crop production index</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -472,6 +472,11 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>13. Population</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)</t>
         </is>
       </c>
     </row>
@@ -482,81 +487,30 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2012</v>
-      </c>
-      <c r="C2" t="n">
-        <v>324000</v>
+        <v>2014</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>106.91</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>27.55</v>
+        <v>27.65</v>
       </c>
       <c r="E2" t="n">
-        <v>59.6712848</v>
+        <v>59.66004283</v>
       </c>
       <c r="F2" t="n">
-        <v>253.3</v>
+        <v>235.09</v>
       </c>
       <c r="G2" t="n">
-        <v>3.327887329</v>
+        <v>4.200625935</v>
       </c>
       <c r="H2" t="n">
-        <v>35159792</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SDN</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C3" t="n">
-        <v>265000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>27.54</v>
-      </c>
-      <c r="E3" t="n">
-        <v>59.66453961</v>
-      </c>
-      <c r="F3" t="n">
-        <v>241.01</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.612458392</v>
-      </c>
-      <c r="H3" t="n">
-        <v>35990704</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>SDN</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C4" t="n">
-        <v>473000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>27.65</v>
-      </c>
-      <c r="E4" t="n">
-        <v>59.66004283</v>
-      </c>
-      <c r="F4" t="n">
-        <v>235.09</v>
-      </c>
-      <c r="G4" t="n">
-        <v>4.200625935</v>
-      </c>
-      <c r="H4" t="n">
         <v>37003245</v>
+      </c>
+      <c r="I2" t="n">
+        <v>43.2859542809493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>